<commit_message>
Text updates as supplied by PM&C.
</commit_message>
<xml_diff>
--- a/dashboard_loader/disability_more_assist_uploader/disability_more_assist.xlsx
+++ b/dashboard_loader/disability_more_assist_uploader/disability_more_assist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t xml:space="preserve">Need for more formal assistance</t>
   </si>
@@ -95,7 +95,10 @@
     <t xml:space="preserve">In 2015, 35.3 per cent of those reporting a disability said they require more formal assistance than they are currently receiving. 78.7 per cent were satisfied with the quality of assistance received from formal services.</t>
   </si>
   <si>
-    <t xml:space="preserve">Nationally, between 2009 and 2015, there was no significant change.. Over this same period, there were increases in all states and territories, except for Queensland and the Australian Capital Territory. Progress will need to improve in order to meet the target.</t>
+    <t xml:space="preserve">Nationally, between 2009 and 2015, there was no significant change in the proportion of people with disability who report a need for more formal assistance. Progress will need to improve in order to meet the target.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All jurisdictions have committed to rolling out the National Disability Insurance Scheme (NDIS) to full scheme.  The NDIS is transforming Australia’s system of support for people with disability through an insurance approach.  The NDIS provides assurance that people with disability will be able to receive care and support over their lifetime based on their needs, and that they will have choice and control over that support. </t>
   </si>
   <si>
     <t xml:space="preserve">Influences</t>
@@ -110,10 +113,10 @@
     <t xml:space="preserve">Excludes those with a need for assistance with health care and people who are residents of cared accommodation. Need for more formal assistance also includes those who currently do not receive any assistance or may not be eligible for assistance.</t>
   </si>
   <si>
-    <t xml:space="preserve">Sourced from: ABS, Survey of Disability, Ageing and Carers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data for the Northern Territory should be used with care as the Survey of Disability, Ageing and Carers does not include people living in very remote areas or people living in discrete Indigenous communities, which affects the comparability of the Northern Territory results.  In addition the 2012 survey was the first time that discrete Indigenous communities were excluded from the survey, resulting in around 10% of Northern Territory households that were previously included being excluded.</t>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABS, Survey of Disability, Ageing and Carers</t>
   </si>
 </sst>
 </file>
@@ -125,11 +128,12 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="########\ ###\ ##0.0;\-########\ ###\ ##0.0;\–"/>
   </numFmts>
-  <fonts count="7">
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+  <fonts count="17">
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -145,6 +149,87 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -159,14 +244,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -175,17 +254,74 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -203,7 +339,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,7 +363,55 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -237,52 +421,128 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="36" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -293,15 +553,15 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="130.790816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="130.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -704,17 +964,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="136.852040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="136.85"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,7 +1009,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
         <v>22</v>
       </c>
@@ -757,46 +1017,47 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="25.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7"/>
       <c r="B6" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+    <row r="7" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="8" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="8" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
       <c r="B9" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>